<commit_message>
Added BR Containers, definition and work on BR Conflats
</commit_message>
<xml_diff>
--- a/docs/SpriteIDs.xlsx
+++ b/docs/SpriteIDs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BRTrains2-Extended\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74897216-E60D-4A3C-998C-C8999083332C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499EC1D3-718D-44A6-9ADA-6B21AA7F123D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="891">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="894">
   <si>
     <t>ID No.</t>
   </si>
@@ -2598,9 +2598,6 @@
     <t>BR_Conflat_A</t>
   </si>
   <si>
-    <t>BR Conflat A</t>
-  </si>
-  <si>
     <t>13 tons</t>
   </si>
   <si>
@@ -2734,6 +2731,18 @@
   </si>
   <si>
     <t>BR Class 37/0 "Tractors" / EE Type 3 - Random Headcode</t>
+  </si>
+  <si>
+    <t>BR_Conflat_P</t>
+  </si>
+  <si>
+    <t>BR Conflat A - Diagram 61/62</t>
+  </si>
+  <si>
+    <t>12 tons</t>
+  </si>
+  <si>
+    <t>BR Conflat P - Diagram 60</t>
   </si>
 </sst>
 </file>
@@ -3225,11 +3234,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3270,491 +3279,513 @@
       <c r="A3">
         <v>500</v>
       </c>
-      <c r="B3" t="s">
-        <v>844</v>
-      </c>
-      <c r="C3" t="s">
-        <v>845</v>
-      </c>
-      <c r="D3">
-        <v>1950</v>
-      </c>
-      <c r="E3" t="s">
-        <v>846</v>
-      </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>501</v>
+      </c>
+      <c r="B4" t="s">
+        <v>844</v>
+      </c>
+      <c r="C4" t="s">
+        <v>891</v>
+      </c>
+      <c r="D4">
+        <v>1950</v>
+      </c>
+      <c r="E4" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>502</v>
+      </c>
+      <c r="B5" t="s">
+        <v>890</v>
+      </c>
+      <c r="C5" t="s">
+        <v>893</v>
+      </c>
+      <c r="D5">
+        <v>1959</v>
+      </c>
+      <c r="E5" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>720</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>842</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>843</v>
       </c>
-      <c r="D4">
+      <c r="D6">
         <v>1952</v>
       </c>
-      <c r="E4" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>3700</v>
-      </c>
-      <c r="B7" t="s">
-        <v>877</v>
-      </c>
-      <c r="C7" t="s">
-        <v>890</v>
-      </c>
-      <c r="D7">
-        <v>1960</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>3701</v>
-      </c>
-      <c r="B8" t="s">
-        <v>885</v>
-      </c>
-      <c r="C8" t="s">
-        <v>886</v>
-      </c>
-      <c r="D8">
-        <v>1977</v>
+      <c r="E6" t="s">
+        <v>846</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>3702</v>
+        <v>3700</v>
       </c>
       <c r="B9" t="s">
-        <v>884</v>
+        <v>876</v>
       </c>
       <c r="C9" t="s">
-        <v>888</v>
+        <v>889</v>
+      </c>
+      <c r="D9">
+        <v>1960</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>3703</v>
+        <v>3701</v>
       </c>
       <c r="B10" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="C10" t="s">
-        <v>889</v>
+        <v>885</v>
+      </c>
+      <c r="D10">
+        <v>1977</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>3710</v>
+        <v>3702</v>
+      </c>
+      <c r="B11" t="s">
+        <v>883</v>
+      </c>
+      <c r="C11" t="s">
+        <v>887</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>3720</v>
+        <v>3703</v>
+      </c>
+      <c r="B12" t="s">
+        <v>886</v>
+      </c>
+      <c r="C12" t="s">
+        <v>888</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>3730</v>
-      </c>
-      <c r="B13" t="s">
-        <v>882</v>
-      </c>
-      <c r="C13" t="s">
-        <v>883</v>
+        <v>3710</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>3740</v>
+        <v>3720</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>3750</v>
+        <v>3730</v>
+      </c>
+      <c r="B15" t="s">
+        <v>881</v>
+      </c>
+      <c r="C15" t="s">
+        <v>882</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16">
+        <v>3740</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>3760</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>3770</v>
-      </c>
-      <c r="B17" t="s">
-        <v>879</v>
-      </c>
-      <c r="C17" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>3780</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>3790</v>
       </c>
       <c r="B19" t="s">
         <v>878</v>
       </c>
       <c r="C19" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>3780</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21">
+        <v>3790</v>
+      </c>
+      <c r="B21" t="s">
+        <v>877</v>
+      </c>
+      <c r="C21" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>3800</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>838</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>839</v>
       </c>
-      <c r="D21">
+      <c r="D23">
         <v>2010</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E23" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>3801</v>
+      </c>
+      <c r="B24" t="s">
+        <v>840</v>
+      </c>
+      <c r="C24" t="s">
+        <v>841</v>
+      </c>
+      <c r="D24">
+        <v>2010</v>
+      </c>
+      <c r="E24" t="s">
         <v>848</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>3801</v>
-      </c>
-      <c r="B22" t="s">
-        <v>840</v>
-      </c>
-      <c r="C22" t="s">
-        <v>841</v>
-      </c>
-      <c r="D22">
-        <v>2010</v>
-      </c>
-      <c r="E22" t="s">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>3802</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>3803</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>3804</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>3805</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>3806</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>3807</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>3808</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>3809</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>3810</v>
+      </c>
+      <c r="B33" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>3802</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>3803</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>3804</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>3805</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>3806</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>3807</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>3808</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>3809</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>3810</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="C33" t="s">
+        <v>851</v>
+      </c>
+      <c r="F33" t="s">
         <v>850</v>
       </c>
-      <c r="C31" t="s">
-        <v>852</v>
-      </c>
-      <c r="F31" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39">
+    </row>
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41">
         <v>4300</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B41" t="s">
+        <v>870</v>
+      </c>
+      <c r="C41" t="s">
         <v>871</v>
       </c>
-      <c r="C39" t="s">
+    </row>
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>4310</v>
+      </c>
+      <c r="B42" t="s">
         <v>872</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>4310</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="C42" t="s">
         <v>873</v>
       </c>
-      <c r="C40" t="s">
+    </row>
+    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>4320</v>
+      </c>
+      <c r="B43" t="s">
         <v>874</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>4320</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="C43" t="s">
         <v>875</v>
       </c>
-      <c r="C41" t="s">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42">
+    </row>
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44">
         <v>4330</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43">
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45">
         <v>4340</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44">
+    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46">
         <v>4350</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45">
+    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47">
         <v>4360</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46">
+    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48">
         <v>4370</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>4380</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>4390</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>4400</v>
-      </c>
-      <c r="B49" t="s">
-        <v>853</v>
-      </c>
-      <c r="C49" t="s">
-        <v>856</v>
+        <v>4380</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>4410</v>
+        <v>4390</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>4420</v>
+        <v>4400</v>
+      </c>
+      <c r="B51" t="s">
+        <v>852</v>
+      </c>
+      <c r="C51" t="s">
+        <v>855</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>4430</v>
+        <v>4410</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>4440</v>
+        <v>4420</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>4450</v>
+        <v>4430</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>4460</v>
-      </c>
-      <c r="B55" t="s">
-        <v>834</v>
-      </c>
-      <c r="C55" t="s">
-        <v>836</v>
-      </c>
-      <c r="D55">
-        <v>1934</v>
+        <v>4440</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>4450</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57">
+        <v>4460</v>
+      </c>
+      <c r="B57" t="s">
+        <v>834</v>
+      </c>
+      <c r="C57" t="s">
+        <v>836</v>
+      </c>
+      <c r="D57">
+        <v>1934</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59">
         <v>4500</v>
       </c>
-      <c r="B57" t="s">
-        <v>855</v>
-      </c>
-      <c r="C57" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>4600</v>
-      </c>
-      <c r="B58" t="s">
-        <v>858</v>
-      </c>
-      <c r="C58" t="s">
-        <v>859</v>
+      <c r="B59" t="s">
+        <v>854</v>
+      </c>
+      <c r="C59" t="s">
+        <v>856</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>4700</v>
+        <v>4600</v>
       </c>
       <c r="B60" t="s">
-        <v>314</v>
+        <v>857</v>
       </c>
       <c r="C60" t="s">
-        <v>866</v>
-      </c>
-      <c r="D60">
-        <v>1962</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>4710</v>
+        <v>858</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>4720</v>
+        <v>4700</v>
+      </c>
+      <c r="B62" t="s">
+        <v>314</v>
+      </c>
+      <c r="C62" t="s">
+        <v>865</v>
+      </c>
+      <c r="D62">
+        <v>1962</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>4730</v>
-      </c>
-      <c r="B63" t="s">
-        <v>867</v>
-      </c>
-      <c r="C63" t="s">
-        <v>868</v>
+        <v>4710</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>4740</v>
-      </c>
-      <c r="B64" t="s">
-        <v>869</v>
-      </c>
-      <c r="C64" t="s">
-        <v>870</v>
+        <v>4720</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>4750</v>
+        <v>4730</v>
+      </c>
+      <c r="B65" t="s">
+        <v>866</v>
+      </c>
+      <c r="C65" t="s">
+        <v>867</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>4760</v>
+        <v>4740</v>
       </c>
       <c r="B66" t="s">
-        <v>860</v>
+        <v>868</v>
       </c>
       <c r="C66" t="s">
-        <v>861</v>
+        <v>869</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>4770</v>
-      </c>
-      <c r="B67" t="s">
-        <v>864</v>
-      </c>
-      <c r="C67" t="s">
-        <v>865</v>
+        <v>4750</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>4780</v>
+        <v>4760</v>
+      </c>
+      <c r="B68" t="s">
+        <v>859</v>
+      </c>
+      <c r="C68" t="s">
+        <v>860</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69">
+        <v>4770</v>
+      </c>
+      <c r="B69" t="s">
+        <v>863</v>
+      </c>
+      <c r="C69" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>4780</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71">
         <v>4790</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B71" t="s">
+        <v>861</v>
+      </c>
+      <c r="C71" t="s">
         <v>862</v>
-      </c>
-      <c r="C69" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>5200</v>
-      </c>
-      <c r="B72" t="s">
-        <v>835</v>
-      </c>
-      <c r="C72" t="s">
-        <v>854</v>
-      </c>
-      <c r="D72">
-        <v>1961</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74">
+        <v>5200</v>
+      </c>
+      <c r="B74" t="s">
+        <v>835</v>
+      </c>
+      <c r="C74" t="s">
+        <v>853</v>
+      </c>
+      <c r="D74">
+        <v>1961</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76">
         <v>6600</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B76" t="s">
         <v>8</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C76" t="s">
         <v>837</v>
       </c>
-      <c r="D74">
+      <c r="D76">
         <v>1998</v>
       </c>
     </row>

</xml_diff>